<commit_message>
fix function call and express resolve
</commit_message>
<xml_diff>
--- a/工作簿1.xlsx
+++ b/工作簿1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cfile\Complier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A398862C-2E9F-4BA3-B681-3E02C7644732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC43E46D-E5F8-4CE9-93C9-DF792B7071A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1180AA46-D987-40C8-ABCE-95FA557D91A2}"/>
+    <workbookView xWindow="4800" yWindow="3375" windowWidth="28800" windowHeight="15345" xr2:uid="{1180AA46-D987-40C8-ABCE-95FA557D91A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -144,12 +144,27 @@
         </r>
       </text>
     </comment>
+    <comment ref="AJ17" authorId="0" shapeId="0" xr:uid="{70CF5667-997F-463A-A964-D4633E8BB40B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>case -&gt;</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="94">
   <si>
     <t>ACTION</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -399,10 +414,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>S7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>if</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -459,10 +470,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>if body1 waiting enter scope</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>waiting ertent if block2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -504,6 +511,34 @@
   </si>
   <si>
     <t>R15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waiting return start or body</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return type get</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enter_parentheses()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce_rparenthese()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R16</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -573,7 +608,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -591,6 +626,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -927,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{323AC86F-B76D-4B04-954E-44A41ABB7C63}">
-  <dimension ref="A1:AN55"/>
+  <dimension ref="A1:AN61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46:R46"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -951,27 +989,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
       <c r="G1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="S1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AI1" s="11" t="s">
+      <c r="AI1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="11"/>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="11"/>
-      <c r="AM1" s="11"/>
-      <c r="AN1" s="11"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -996,10 +1034,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>12</v>
@@ -1017,12 +1055,15 @@
         <v>60</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="R2" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="S2" s="1">
         <v>0</v>
       </c>
@@ -1116,11 +1157,17 @@
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="H5" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R5" s="8"/>
       <c r="S5" s="1">
@@ -1204,7 +1251,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1283,15 +1330,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>14</v>
       </c>
       <c r="AI17" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AJ17" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1311,10 +1361,10 @@
         <v>61</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AB18" s="6">
         <v>15</v>
@@ -1323,7 +1373,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1337,7 +1387,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1351,18 +1401,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>18</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1373,7 +1423,7 @@
         <v>19</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>19</v>
@@ -1382,45 +1432,45 @@
         <v>61</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P22" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>20</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-    </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B23" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>21</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1436,7 +1486,7 @@
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J25" s="10" t="s">
         <v>19</v>
@@ -1448,13 +1498,13 @@
         <v>61</v>
       </c>
       <c r="O25" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10">
         <v>23</v>
       </c>
@@ -1468,617 +1518,700 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10">
         <v>24</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>0</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="1">
-        <v>0</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
-    </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>1</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="1">
-        <v>1</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>2</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="1">
-        <v>2</v>
-      </c>
-      <c r="G33" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="10">
         <v>26</v>
       </c>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
+      <c r="C29" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>27</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>3</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
       <c r="F34" s="1">
-        <v>3</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>4</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
       <c r="F35" s="1">
-        <v>4</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>5</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
       <c r="F36" s="1">
-        <v>5</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>6</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
       <c r="F37" s="1">
-        <v>6</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="12"/>
+      <c r="Q37" s="12"/>
+      <c r="R37" s="12"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>7</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
       <c r="F38" s="1">
-        <v>7</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="11"/>
-      <c r="R38" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="12"/>
+      <c r="Q38" s="12"/>
+      <c r="R38" s="12"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>8</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
+        <v>5</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
       <c r="F39" s="1">
-        <v>8</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="11"/>
+        <v>5</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="12"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="12"/>
+      <c r="P39" s="12"/>
+      <c r="Q39" s="12"/>
+      <c r="R39" s="12"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>9</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
       <c r="F40" s="1">
-        <v>9</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
+      <c r="N40" s="12"/>
+      <c r="O40" s="12"/>
+      <c r="P40" s="12"/>
+      <c r="Q40" s="12"/>
+      <c r="R40" s="12"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>10</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
       <c r="F41" s="1">
-        <v>10</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="12"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>11</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
+        <v>8</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
       <c r="F42" s="1">
-        <v>11</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
+        <v>8</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="12"/>
+      <c r="N42" s="12"/>
+      <c r="O42" s="12"/>
+      <c r="P42" s="12"/>
+      <c r="Q42" s="12"/>
+      <c r="R42" s="12"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>12</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
       <c r="F43" s="1">
-        <v>12</v>
-      </c>
-      <c r="G43" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="12"/>
+      <c r="N43" s="12"/>
+      <c r="O43" s="12"/>
+      <c r="P43" s="12"/>
+      <c r="Q43" s="12"/>
+      <c r="R43" s="12"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>13</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
       <c r="F44" s="1">
-        <v>13</v>
-      </c>
-      <c r="G44" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="11"/>
-      <c r="L44" s="11"/>
-      <c r="M44" s="11"/>
-      <c r="N44" s="11"/>
-      <c r="O44" s="11"/>
-      <c r="P44" s="11"/>
-      <c r="Q44" s="11"/>
-      <c r="R44" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
+      <c r="N44" s="12"/>
+      <c r="O44" s="12"/>
+      <c r="P44" s="12"/>
+      <c r="Q44" s="12"/>
+      <c r="R44" s="12"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>14</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
       <c r="F45" s="1">
-        <v>14</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>15</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
       <c r="F46" s="1">
-        <v>15</v>
-      </c>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
+      <c r="P46" s="12"/>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="12"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>16</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="1">
+        <v>13</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+      <c r="O47" s="12"/>
+      <c r="P47" s="12"/>
+      <c r="Q47" s="12"/>
+      <c r="R47" s="12"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
+        <v>14</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="1">
+        <v>14</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="12"/>
+      <c r="M48" s="12"/>
+      <c r="N48" s="12"/>
+      <c r="O48" s="12"/>
+      <c r="P48" s="12"/>
+      <c r="Q48" s="12"/>
+      <c r="R48" s="12"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>15</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="1">
+        <v>15</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="12"/>
+      <c r="L49" s="12"/>
+      <c r="M49" s="12"/>
+      <c r="N49" s="12"/>
+      <c r="O49" s="12"/>
+      <c r="P49" s="12"/>
+      <c r="Q49" s="12"/>
+      <c r="R49" s="12"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>16</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="1">
+        <v>16</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
+      <c r="L50" s="12"/>
+      <c r="M50" s="12"/>
+      <c r="N50" s="12"/>
+      <c r="O50" s="12"/>
+      <c r="P50" s="12"/>
+      <c r="Q50" s="12"/>
+      <c r="R50" s="12"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
         <v>17</v>
       </c>
-      <c r="B48" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
+      <c r="B51" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
         <v>18</v>
       </c>
-      <c r="B49" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
         <v>19</v>
       </c>
-      <c r="B50" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
-        <v>20</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
-        <v>21</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
-        <v>22</v>
-      </c>
       <c r="B53" s="12" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
+        <v>20</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>21</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>22</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
         <v>23</v>
       </c>
-      <c r="B54" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
+      <c r="B57" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
         <v>24</v>
       </c>
-      <c r="B55" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
+      <c r="B58" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+    </row>
+    <row r="59" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="11">
+        <v>25</v>
+      </c>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>26</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>27</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="48">
+    <mergeCell ref="G50:R50"/>
+    <mergeCell ref="AI1:AN1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G35:R35"/>
+    <mergeCell ref="G36:R36"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="G34:R34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B23:O23"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="G40:R40"/>
+    <mergeCell ref="G37:R37"/>
+    <mergeCell ref="G38:R38"/>
+    <mergeCell ref="G39:R39"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="G41:R41"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="G42:R42"/>
+    <mergeCell ref="G43:R43"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="G44:R44"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="G45:R45"/>
+    <mergeCell ref="G48:R48"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="G46:R46"/>
+    <mergeCell ref="G47:R47"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B51:E51"/>
     <mergeCell ref="B52:E52"/>
     <mergeCell ref="B53:E53"/>
-    <mergeCell ref="G45:R45"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B50:E50"/>
     <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="G46:R46"/>
-    <mergeCell ref="AI1:AN1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G32:R32"/>
-    <mergeCell ref="G33:R33"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="G31:R31"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B23:O23"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="G37:R37"/>
-    <mergeCell ref="G34:R34"/>
-    <mergeCell ref="G35:R35"/>
-    <mergeCell ref="G36:R36"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="G43:R43"/>
-    <mergeCell ref="G44:R44"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="G38:R38"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="G39:R39"/>
-    <mergeCell ref="G40:R40"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="G41:R41"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="G42:R42"/>
+    <mergeCell ref="G49:R49"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>